<commit_message>
documentos revisados para reporte de monitoreo
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1387 - RNCNOM, Gabriela_OC/Planeación/Plan_de_proyecto.xlsx
+++ b/Proyectos/2015/12/P1387 - RNCNOM, Gabriela_OC/Planeación/Plan_de_proyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Presentación" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,6 +32,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$20</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -159,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="156">
   <si>
     <t>Plan del Proyecto</t>
   </si>
@@ -267,9 +268,6 @@
   </si>
   <si>
     <t>Carta de aceptación</t>
-  </si>
-  <si>
-    <t>5 Notificaciones y no tuvimos respuesta</t>
   </si>
   <si>
     <t>Ciclo de Vida</t>
@@ -1808,15 +1806,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
+      <xdr:colOff>796320</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1825,8 +1823,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10035720" cy="9200880"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="10035360" cy="9200520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1853,15 +1851,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
+      <xdr:colOff>796320</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1870,8 +1868,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10035720" cy="9200880"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="10035360" cy="9200520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1898,15 +1896,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>769680</xdr:colOff>
+      <xdr:colOff>796320</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1915,8 +1913,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10035720" cy="9200880"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="10035360" cy="9200520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1948,15 +1946,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
+      <xdr:colOff>739080</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1965,8 +1963,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="10010160"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="10037160" cy="10009800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1993,15 +1991,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
+      <xdr:colOff>739080</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2010,8 +2008,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="10010160"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="10037160" cy="10009800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2038,15 +2036,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
+      <xdr:colOff>739080</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2055,8 +2053,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="10010160"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="10037160" cy="10009800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2083,15 +2081,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
+      <xdr:colOff>739080</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2100,8 +2098,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="10037520" cy="10010160"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="10037160" cy="10009800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2135,7 +2133,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2273,7 +2271,7 @@
   <dimension ref="A1:AMI30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -4497,7 +4495,7 @@
         <v>42359</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="18" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A18" s="16" t="s">
         <v>34</v>
       </c>
@@ -4506,10 +4504,10 @@
       </c>
       <c r="C18" s="17" t="n">
         <f aca="true">TODAY()</f>
-        <v>42373</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>36</v>
+        <v>42393</v>
+      </c>
+      <c r="D18" s="18" t="n">
+        <v>42388</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
@@ -4537,7 +4535,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="13"/>
@@ -4551,39 +4549,39 @@
     </row>
     <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="53.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="25"/>
     </row>
@@ -4641,7 +4639,7 @@
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27"/>
       <c r="B1" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -4649,7 +4647,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -4658,41 +4656,41 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="C3" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="E3" s="32" t="s">
         <v>49</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="E4" s="35" t="s">
         <v>53</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>8</v>
@@ -4701,66 +4699,66 @@
         <v>3313482553</v>
       </c>
       <c r="D5" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>56</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="C6" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="D6" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="E6" s="36" t="s">
         <v>61</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="33" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="C7" s="33" t="n">
         <v>3318039095</v>
       </c>
       <c r="D7" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="36" t="s">
         <v>65</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="C8" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="D8" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="E8" s="36" t="s">
         <v>70</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>11</v>
@@ -4769,10 +4767,10 @@
         <v>3312448000</v>
       </c>
       <c r="D9" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="36" t="s">
         <v>73</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4791,7 +4789,7 @@
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="37"/>
@@ -4800,19 +4798,19 @@
     </row>
     <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>76</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>77</v>
       </c>
       <c r="C13" s="33" t="n">
         <v>3318144411</v>
       </c>
       <c r="D13" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="38" t="s">
         <v>78</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4843,9 +4841,30 @@
       <c r="D17" s="39"/>
       <c r="E17" s="40"/>
     </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+    </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="41"/>
       <c r="C21" s="41"/>
@@ -4859,7 +4878,7 @@
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="42"/>
       <c r="B23" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -4905,26 +4924,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="C1" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="E1" s="45" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="46"/>
       <c r="B2" s="46"/>
       <c r="C2" s="47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="48"/>
       <c r="E2" s="48"/>
@@ -5004,8 +5023,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -6102,7 +6121,7 @@
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -7129,19 +7148,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="C3" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="52" t="s">
+      <c r="E3" s="52" t="s">
         <v>91</v>
-      </c>
-      <c r="E3" s="52" t="s">
-        <v>92</v>
       </c>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -8164,70 +8183,70 @@
     </row>
     <row r="4" s="56" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="C4" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="D4" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="E4" s="54" t="s">
         <v>96</v>
-      </c>
-      <c r="E4" s="54" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" s="56" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>99</v>
-      </c>
       <c r="E5" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" s="56" customFormat="true" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="55" t="s">
+      <c r="D6" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="E6" s="54" t="s">
         <v>102</v>
-      </c>
-      <c r="E6" s="54" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" s="56" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="E7" s="54" t="s">
         <v>105</v>
-      </c>
-      <c r="E7" s="54" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" s="56" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8280,7 +8299,7 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -8311,7 +8330,7 @@
     </row>
     <row r="2" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -8323,37 +8342,37 @@
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>113</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>114</v>
       </c>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>116</v>
-      </c>
       <c r="C4" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="38" t="n">
         <v>1</v>
@@ -8362,24 +8381,24 @@
         <v>42335</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="60" t="s">
         <v>117</v>
-      </c>
-      <c r="J4" s="60" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>120</v>
-      </c>
       <c r="C5" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="38" t="n">
         <v>2</v>
@@ -8388,13 +8407,13 @@
         <v>42335</v>
       </c>
       <c r="F5" s="59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J5" s="60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8548,7 +8567,7 @@
       <c r="C2" s="66"/>
       <c r="D2" s="66"/>
       <c r="E2" s="65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F2" s="66"/>
       <c r="G2" s="66"/>
@@ -8557,7 +8576,7 @@
       <c r="J2" s="66"/>
       <c r="K2" s="67"/>
       <c r="IR2" s="68" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="IS2" s="68"/>
       <c r="IT2" s="68"/>
@@ -8582,51 +8601,51 @@
       <c r="J3" s="72"/>
       <c r="K3" s="73"/>
       <c r="AE3" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF3" s="74" t="s">
         <v>124</v>
-      </c>
-      <c r="AF3" s="74" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="C4" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="D4" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="E4" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="F4" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="G4" s="77" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="H4" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="I4" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="I4" s="77" t="s">
+      <c r="J4" s="78" t="s">
         <v>134</v>
       </c>
-      <c r="J4" s="78" t="s">
+      <c r="K4" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="K4" s="77" t="s">
-        <v>136</v>
-      </c>
       <c r="AE4" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF4" s="79" t="s">
         <v>124</v>
-      </c>
-      <c r="AF4" s="79" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8634,7 +8653,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C5" s="80" t="n">
         <v>5</v>
@@ -8650,19 +8669,19 @@
         <v>4</v>
       </c>
       <c r="G5" s="81" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="81" t="s">
         <v>138</v>
-      </c>
-      <c r="H5" s="81" t="s">
-        <v>139</v>
       </c>
       <c r="I5" s="80" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="83" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K5" s="84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="IS5" s="85"/>
       <c r="IT5" s="86"/>
@@ -8678,7 +8697,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" s="80" t="n">
         <v>5</v>
@@ -8694,25 +8713,25 @@
         <v>4</v>
       </c>
       <c r="G6" s="81" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="81" t="s">
         <v>142</v>
-      </c>
-      <c r="H6" s="81" t="s">
-        <v>143</v>
       </c>
       <c r="I6" s="80" t="s">
         <v>11</v>
       </c>
       <c r="J6" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="K6" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="IS6" s="90" t="s">
         <v>144</v>
       </c>
-      <c r="K6" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="IS6" s="90" t="s">
+      <c r="IT6" s="91" t="s">
         <v>145</v>
-      </c>
-      <c r="IT6" s="91" t="s">
-        <v>146</v>
       </c>
       <c r="IU6" s="92" t="n">
         <v>0.9</v>
@@ -8757,7 +8776,7 @@
       <c r="K7" s="101"/>
       <c r="IS7" s="90"/>
       <c r="IT7" s="91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="IU7" s="92" t="n">
         <v>0.5</v>
@@ -8802,7 +8821,7 @@
       <c r="K8" s="101"/>
       <c r="IS8" s="90"/>
       <c r="IT8" s="91" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="IU8" s="92" t="n">
         <v>0.3</v>
@@ -8847,7 +8866,7 @@
       <c r="K9" s="101"/>
       <c r="IS9" s="90"/>
       <c r="IT9" s="91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="IU9" s="110" t="n">
         <v>0.1</v>
@@ -8930,19 +8949,19 @@
       <c r="IT11" s="123"/>
       <c r="IU11" s="123"/>
       <c r="IV11" s="91" t="s">
+        <v>146</v>
+      </c>
+      <c r="IW11" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="IW11" s="91" t="s">
+      <c r="IX11" s="91" t="s">
         <v>148</v>
       </c>
-      <c r="IX11" s="91" t="s">
+      <c r="IY11" s="91" t="s">
         <v>149</v>
       </c>
-      <c r="IY11" s="91" t="s">
-        <v>150</v>
-      </c>
       <c r="IZ11" s="125" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8966,7 +8985,7 @@
       <c r="IT12" s="123"/>
       <c r="IU12" s="92"/>
       <c r="IV12" s="126" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="IW12" s="126"/>
       <c r="IX12" s="126"/>
@@ -9043,7 +9062,7 @@
       <c r="J15" s="120"/>
       <c r="K15" s="121"/>
       <c r="IS15" s="130" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="IT15" s="130"/>
       <c r="IU15" s="128"/>
@@ -9071,12 +9090,12 @@
       <c r="J16" s="120"/>
       <c r="K16" s="121"/>
       <c r="IS16" s="131" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="IT16" s="132"/>
       <c r="IU16" s="128"/>
       <c r="IV16" s="133" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="IW16" s="133"/>
       <c r="IX16" s="133"/>
@@ -9101,12 +9120,12 @@
       <c r="J17" s="120"/>
       <c r="K17" s="121"/>
       <c r="IS17" s="131" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="IT17" s="134"/>
       <c r="IU17" s="128"/>
       <c r="IV17" s="133" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="IW17" s="133"/>
       <c r="IX17" s="133"/>
@@ -9131,12 +9150,12 @@
       <c r="J18" s="120"/>
       <c r="K18" s="121"/>
       <c r="IS18" s="131" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="IT18" s="135"/>
       <c r="IU18" s="128"/>
       <c r="IV18" s="133" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="IW18" s="133"/>
       <c r="IX18" s="133"/>

</xml_diff>